<commit_message>
feat: adds random forest regression results and set PLSR results
</commit_message>
<xml_diff>
--- a/Partial Least Squares Regression/PLSR_metrics_MSC.xlsx
+++ b/Partial Least Squares Regression/PLSR_metrics_MSC.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,16 +472,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6772065512993893</v>
+        <v>0.751126762567406</v>
       </c>
       <c r="C2" t="n">
-        <v>1.337606135248314</v>
+        <v>1.174505337654611</v>
       </c>
       <c r="D2" t="n">
-        <v>4.158297550000612</v>
+        <v>3.069342633011423</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7064698067530116</v>
+        <v>0.7851754730668938</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -496,16 +496,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7172527101422645</v>
+        <v>0.8392668032967503</v>
       </c>
       <c r="C3" t="n">
-        <v>1.251886976972629</v>
+        <v>0.9438841367466636</v>
       </c>
       <c r="D3" t="n">
-        <v>4.025998267814308</v>
+        <v>2.28865702597232</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7172527101422651</v>
+        <v>0.8392668032967507</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -520,16 +520,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6772097355071809</v>
+        <v>0.7843807409086087</v>
       </c>
       <c r="C4" t="n">
-        <v>1.553545515389507</v>
+        <v>1.269718778002052</v>
       </c>
       <c r="D4" t="n">
-        <v>-4.855944328159742</v>
+        <v>-3.285878779254537</v>
       </c>
       <c r="E4" t="n">
-        <v>1.339393823261507</v>
+        <v>1.230075841862674</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -544,16 +544,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2749903227257471</v>
+        <v>0.3356296506909373</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2608279062550376</v>
+        <v>0.2496820229151687</v>
       </c>
       <c r="D5" t="n">
-        <v>2.075413498971369</v>
+        <v>1.743425413331221</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3686585602088941</v>
+        <v>0.4709357672430803</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -568,16 +568,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.439798594032087</v>
+        <v>0.5479003523073099</v>
       </c>
       <c r="C6" t="n">
-        <v>0.229273705819987</v>
+        <v>0.2059677561491342</v>
       </c>
       <c r="D6" t="n">
-        <v>1.840924256839081</v>
+        <v>1.485682111968045</v>
       </c>
       <c r="E6" t="n">
-        <v>0.439798594032087</v>
+        <v>0.5479003523073097</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -592,16 +592,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5293543830861951</v>
+        <v>0.5986207557863301</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1847057507674995</v>
+        <v>0.1705732261062677</v>
       </c>
       <c r="D7" t="n">
-        <v>-1.035733885148385</v>
+        <v>-0.6075403084347162</v>
       </c>
       <c r="E7" t="n">
-        <v>1.305885888547491</v>
+        <v>1.18285999528346</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -616,16 +616,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5502862862348172</v>
+        <v>0.5982023189954349</v>
       </c>
       <c r="C8" t="n">
-        <v>1.998762783762816</v>
+        <v>1.889282499519987</v>
       </c>
       <c r="D8" t="n">
-        <v>6.229955109554997</v>
+        <v>5.246821010190581</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6004757473760328</v>
+        <v>0.663270628283821</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -640,16 +640,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.6169608592912119</v>
+        <v>0.7381685387562533</v>
       </c>
       <c r="C9" t="n">
-        <v>1.844653354678704</v>
+        <v>1.525120306145279</v>
       </c>
       <c r="D9" t="n">
-        <v>5.976846147206121</v>
+        <v>4.085552086025035</v>
       </c>
       <c r="E9" t="n">
-        <v>0.61696085929121</v>
+        <v>0.7381685387562533</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -664,16 +664,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.7582214349932668</v>
+        <v>0.8413985933904321</v>
       </c>
       <c r="C10" t="n">
-        <v>1.337510928376801</v>
+        <v>1.08328307709383</v>
       </c>
       <c r="D10" t="n">
-        <v>-2.594691716283135</v>
+        <v>-0.3372503031000456</v>
       </c>
       <c r="E10" t="n">
-        <v>1.161241625570269</v>
+        <v>1.01768351548744</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -688,16 +688,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3869386133289522</v>
+        <v>0.3718699914299578</v>
       </c>
       <c r="C11" t="n">
-        <v>75.06886367733406</v>
+        <v>75.98583345497205</v>
       </c>
       <c r="D11" t="n">
-        <v>274.6456242887231</v>
+        <v>261.708078076195</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4548476885247753</v>
+        <v>0.4744101715212649</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -712,16 +712,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.5054071733614569</v>
+        <v>0.5476973011871675</v>
       </c>
       <c r="C12" t="n">
-        <v>67.42667858376628</v>
+        <v>64.47961711507432</v>
       </c>
       <c r="D12" t="n">
-        <v>248.7918161437354</v>
+        <v>227.51888790857</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5054071733614574</v>
+        <v>0.5476973011871683</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -736,16 +736,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.6132002975129864</v>
+        <v>0.5692874832349819</v>
       </c>
       <c r="C13" t="n">
-        <v>58.64777071923054</v>
+        <v>61.88739312795758</v>
       </c>
       <c r="D13" t="n">
-        <v>-22.06078538207953</v>
+        <v>29.05588005621365</v>
       </c>
       <c r="E13" t="n">
-        <v>1.042559720594414</v>
+        <v>0.9443671757127473</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -760,16 +760,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3827984091554695</v>
+        <v>0.4357359037190185</v>
       </c>
       <c r="C14" t="n">
-        <v>0.363270989530245</v>
+        <v>0.3473428849905844</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5543431152833778</v>
+        <v>0.4631455524918358</v>
       </c>
       <c r="E14" t="n">
-        <v>0.471051661521707</v>
+        <v>0.5566831898667799</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -784,16 +784,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.5275499970941053</v>
+        <v>0.6991188334340346</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3178301746254875</v>
+        <v>0.2536382222984024</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4895202964394602</v>
+        <v>0.311752432944231</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5275499970941057</v>
+        <v>0.6991188334340357</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -808,378 +808,18 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.4134830982500701</v>
+        <v>0.4838827585769574</v>
       </c>
       <c r="C16" t="n">
-        <v>0.511706388260915</v>
+        <v>0.4800149422733923</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.369622705504713</v>
+        <v>-0.1630039435739303</v>
       </c>
       <c r="E16" t="n">
-        <v>1.415628284920585</v>
+        <v>1.177670595505637</v>
       </c>
       <c r="F16" t="inlineStr">
-        <is>
-          <t>AT</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Referência</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0.7589228508246069</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1.155962963539641</v>
-      </c>
-      <c r="D17" t="n">
-        <v>2.063311428090442</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.8550244587999996</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>SST</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>CV</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0.9330042583098572</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.6093818232703851</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.9539427951056886</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.9330042583098583</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>SST</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Validação</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>0.8176781752232735</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1.167570456138351</v>
-      </c>
-      <c r="D19" t="n">
-        <v>-2.804291077633694</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1.195408380566173</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>SST</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Referência</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0.3356296506909373</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.2496820229151687</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1.743425413331221</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.4709357672430803</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>PH</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>CV</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0.5479003523073099</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.2059677561491342</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1.485682111968045</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.5479003523073097</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>PH</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Validação</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.5986207557863301</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.1705732261062677</v>
-      </c>
-      <c r="D22" t="n">
-        <v>-0.6075403084347162</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1.18285999528346</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>PH</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Referência</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>0.5439632801997134</v>
-      </c>
-      <c r="C23" t="n">
-        <v>2.012765108892804</v>
-      </c>
-      <c r="D23" t="n">
-        <v>4.298469689467727</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.7234002649320267</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>UBS (%)</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>CV</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>0.830994972566715</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1.225301600263165</v>
-      </c>
-      <c r="D24" t="n">
-        <v>2.637111824143991</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.8309949725667133</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>UBS (%)</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Validação</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>0.8733673574045103</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.967968615366003</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.8808766759598772</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.9342983559002197</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>UBS (%)</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Referência</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>0.2897439264220095</v>
-      </c>
-      <c r="C26" t="n">
-        <v>80.80074004717314</v>
-      </c>
-      <c r="D26" t="n">
-        <v>258.7292931664204</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.4860910419641741</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>FIRMEZA (N)</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>CV</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>0.6714045284851271</v>
-      </c>
-      <c r="C27" t="n">
-        <v>54.95897790409411</v>
-      </c>
-      <c r="D27" t="n">
-        <v>165.2912451044055</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.6714045284851277</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>FIRMEZA (N)</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Validação</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>0.5448672004747698</v>
-      </c>
-      <c r="C28" t="n">
-        <v>63.61763355013672</v>
-      </c>
-      <c r="D28" t="n">
-        <v>87.18567802533568</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.8327586680714976</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>FIRMEZA (N)</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Referência</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>0.4322890541069242</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.3484021548464503</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0.4095087091389393</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.6137686492776203</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>AT</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>CV</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>0.8171398363433098</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0.1977319050404477</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0.1894671625984119</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.8171398363433098</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>AT</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Validação</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>0.4930917146893903</v>
-      </c>
-      <c r="C31" t="n">
-        <v>0.4757132717636903</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0.0030517096881435</v>
-      </c>
-      <c r="E31" t="n">
-        <v>1.049520076189464</v>
-      </c>
-      <c r="F31" t="inlineStr">
         <is>
           <t>AT</t>
         </is>

</xml_diff>

<commit_message>
feat: implements svmr notebook and add standardscaler to plsr main
</commit_message>
<xml_diff>
--- a/Partial Least Squares Regression/PLSR_metrics_MSC.xlsx
+++ b/Partial Least Squares Regression/PLSR_metrics_MSC.xlsx
@@ -472,16 +472,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.751126762567406</v>
+        <v>0.7511267625674056</v>
       </c>
       <c r="C2" t="n">
-        <v>1.174505337654611</v>
+        <v>1.174505337654612</v>
       </c>
       <c r="D2" t="n">
-        <v>3.069342633011423</v>
+        <v>3.069342633011421</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7851754730668938</v>
+        <v>0.7851754730668936</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -502,10 +502,10 @@
         <v>0.9438841367466636</v>
       </c>
       <c r="D3" t="n">
-        <v>2.28865702597232</v>
+        <v>2.288657025972322</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8392668032967507</v>
+        <v>0.8392668032967509</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -520,16 +520,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7843807409086087</v>
+        <v>0.6947032220235132</v>
       </c>
       <c r="C4" t="n">
-        <v>1.269718778002052</v>
+        <v>1.510862277990596</v>
       </c>
       <c r="D4" t="n">
-        <v>-3.285878779254537</v>
+        <v>-0.1663351976388032</v>
       </c>
       <c r="E4" t="n">
-        <v>1.230075841862674</v>
+        <v>0.953330387505735</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -550,10 +550,10 @@
         <v>0.2496820229151687</v>
       </c>
       <c r="D5" t="n">
-        <v>1.743425413331221</v>
+        <v>1.743425413331225</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4709357672430803</v>
+        <v>0.4709357672430788</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -568,7 +568,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5479003523073099</v>
+        <v>0.54790035230731</v>
       </c>
       <c r="C6" t="n">
         <v>0.2059677561491342</v>
@@ -577,7 +577,7 @@
         <v>1.485682111968045</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5479003523073097</v>
+        <v>0.5479003523073096</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -592,16 +592,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5986207557863301</v>
+        <v>0.4350736390815085</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1705732261062677</v>
+        <v>0.2023621702127827</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.6075403084347162</v>
+        <v>0.3979485974093362</v>
       </c>
       <c r="E7" t="n">
-        <v>1.18285999528346</v>
+        <v>0.8793012627533111</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -616,16 +616,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5982023189954349</v>
+        <v>0.5982023189954352</v>
       </c>
       <c r="C8" t="n">
-        <v>1.889282499519987</v>
+        <v>1.889282499519986</v>
       </c>
       <c r="D8" t="n">
-        <v>5.246821010190581</v>
+        <v>5.246821010190586</v>
       </c>
       <c r="E8" t="n">
-        <v>0.663270628283821</v>
+        <v>0.6632706282838209</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -646,10 +646,10 @@
         <v>1.525120306145279</v>
       </c>
       <c r="D9" t="n">
-        <v>4.085552086025035</v>
+        <v>4.085552086025032</v>
       </c>
       <c r="E9" t="n">
-        <v>0.7381685387562533</v>
+        <v>0.7381685387562538</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -664,16 +664,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8413985933904321</v>
+        <v>0.6269980998833792</v>
       </c>
       <c r="C10" t="n">
-        <v>1.08328307709383</v>
+        <v>1.661284310198333</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.3372503031000456</v>
+        <v>2.117509708730804</v>
       </c>
       <c r="E10" t="n">
-        <v>1.01768351548744</v>
+        <v>0.798964843940331</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -688,16 +688,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3718699914299578</v>
+        <v>0.3718699914299579</v>
       </c>
       <c r="C11" t="n">
-        <v>75.98583345497205</v>
+        <v>75.98583345497204</v>
       </c>
       <c r="D11" t="n">
-        <v>261.708078076195</v>
+        <v>261.7080780761954</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4744101715212649</v>
+        <v>0.4744101715212642</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -712,16 +712,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.5476973011871675</v>
+        <v>0.5476973011871676</v>
       </c>
       <c r="C12" t="n">
         <v>64.47961711507432</v>
       </c>
       <c r="D12" t="n">
-        <v>227.51888790857</v>
+        <v>227.5188879085707</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5476973011871683</v>
+        <v>0.5476973011871671</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -736,16 +736,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5692874832349819</v>
+        <v>0.4515593679468755</v>
       </c>
       <c r="C13" t="n">
-        <v>61.88739312795758</v>
+        <v>69.83501878436971</v>
       </c>
       <c r="D13" t="n">
-        <v>29.05588005621365</v>
+        <v>140.3680615770823</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9443671757127473</v>
+        <v>0.765628649361459</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -760,13 +760,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.4357359037190185</v>
+        <v>0.4357359037190183</v>
       </c>
       <c r="C14" t="n">
         <v>0.3473428849905844</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4631455524918358</v>
+        <v>0.4631455524918361</v>
       </c>
       <c r="E14" t="n">
         <v>0.5566831898667799</v>
@@ -784,16 +784,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.6991188334340346</v>
+        <v>0.6991188334340351</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2536382222984024</v>
+        <v>0.2536382222984022</v>
       </c>
       <c r="D15" t="n">
-        <v>0.311752432944231</v>
+        <v>0.3117524329442313</v>
       </c>
       <c r="E15" t="n">
-        <v>0.6991188334340357</v>
+        <v>0.699118833434035</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -808,16 +808,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.4838827585769574</v>
+        <v>0.3055639137124027</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4800149422733923</v>
+        <v>0.5567967778383045</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.1630039435739303</v>
+        <v>0.08942439561234861</v>
       </c>
       <c r="E16" t="n">
-        <v>1.177670595505637</v>
+        <v>1.168541207869414</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>

</xml_diff>